<commit_message>
Downloaded data from API.
</commit_message>
<xml_diff>
--- a/plos_fields_fl.xlsx
+++ b/plos_fields_fl.xlsx
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +938,7 @@
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>